<commit_message>
continue v2 tc execution
</commit_message>
<xml_diff>
--- a/IntegrationPlanning.xlsx
+++ b/IntegrationPlanning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Python-Hub\GithubRepos\Guru99-SW-Tesing-Project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D8342F-CB6D-4E64-B710-54610213C237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023B414C-1F64-48EE-A3DD-DDFB6878A0E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4110" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="100">
   <si>
     <t>Date</t>
   </si>
@@ -60,12 +60,6 @@
   </si>
   <si>
     <t>Expected Result</t>
-  </si>
-  <si>
-    <t>Actual Result</t>
-  </si>
-  <si>
-    <t>Pass/Fail</t>
   </si>
   <si>
     <t>IP1</t>
@@ -327,12 +321,39 @@
   <si>
     <t>Fail</t>
   </si>
+  <si>
+    <t>Actual Result v1</t>
+  </si>
+  <si>
+    <t>Pass/Fail  v1</t>
+  </si>
+  <si>
+    <t>Actual Result  v2</t>
+  </si>
+  <si>
+    <t>Pass/Fail v2</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Not authourized</t>
+  </si>
+  <si>
+    <t>Message displayed"Email address already exist"</t>
+  </si>
+  <si>
+    <t>Account does not exist</t>
+  </si>
+  <si>
+    <t>You are not authorize to delete this customer!!</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -378,8 +399,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -407,6 +435,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -600,11 +633,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -656,111 +690,115 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1187,10 +1225,10 @@
         <v>1</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1724,7 +1762,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1735,8 +1773,11 @@
     <col min="4" max="4" width="38" style="14" customWidth="1"/>
     <col min="5" max="5" width="40.28515625" style="14" customWidth="1"/>
     <col min="6" max="6" width="33" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="15.140625" style="14"/>
+    <col min="7" max="7" width="3.5703125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="50" customWidth="1"/>
+    <col min="9" max="9" width="36.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" style="50" customWidth="1"/>
+    <col min="11" max="16384" width="15.140625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="28.5" x14ac:dyDescent="0.2">
@@ -1759,13 +1800,17 @@
         <v>11</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
+        <v>91</v>
+      </c>
+      <c r="H1" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>94</v>
+      </c>
       <c r="K1" s="13"/>
       <c r="L1" s="13"/>
       <c r="M1" s="13"/>
@@ -1777,467 +1822,575 @@
       <c r="S1" s="13"/>
       <c r="T1" s="13"/>
     </row>
-    <row r="2" spans="1:20" s="21" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="141" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="D2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="E2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="F2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="G2" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="J2" s="45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="23" customFormat="1" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" s="26" customFormat="1" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="D3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="22" t="s">
+      <c r="E3" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="G3" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="J3" s="51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="26" customFormat="1" ht="141" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="22" t="s">
+      <c r="B4" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" s="29" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+      <c r="C4" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="D4" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="G4" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="J4" s="45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="27" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="H4" s="43" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" s="21" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="D5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="15" t="s">
+      <c r="F5" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="15" t="s">
+      <c r="G5" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="J5" s="49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="23" customFormat="1" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" s="26" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="D6" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="22" t="s">
+      <c r="E6" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="F6" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="G6" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="J6" s="49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" s="30" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="B7" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="H6" s="44" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" s="33" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="C7" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="D7" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="F7" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="32" t="s">
+      <c r="G7" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7" s="49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" s="31" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="B8" s="28"/>
+      <c r="C8" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="H7" s="46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" s="34" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+      <c r="D8" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="30" t="s">
+      <c r="E8" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="J8" s="49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" s="35" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="B9" s="33"/>
+      <c r="C9" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" s="38" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="D9" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="35" t="s">
+      <c r="E9" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="F9" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="G9" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="J9" s="49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="B10" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="H9" s="44" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" s="21" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="D10" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="E10" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="F10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="G10" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" s="49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" s="23" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="H10" s="49" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" s="26" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="D11" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="J11" s="49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="22" t="s">
+      <c r="B12" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="H11" s="25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" s="21" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="D12" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="G12" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" s="49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="F12" s="19" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="H12" s="49" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" s="21" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
+      <c r="D13" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="15" t="s">
+      <c r="G13" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H13" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="J13" s="49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="F13" s="15" t="s">
+      <c r="B14" s="17"/>
+      <c r="C14" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="G13" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" s="21" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+      <c r="D14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="I14" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="J14" s="51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" s="35" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="15" t="s">
+      <c r="B15" s="33"/>
+      <c r="C15" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" s="38" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="D15" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="35" t="s">
+      <c r="E15" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="F15" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="G15" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="I15" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="J15" s="49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="35" t="s">
+      <c r="B16" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="H15" s="50" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" s="21" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
+      <c r="C16" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="D16" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="F16" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="19" t="s">
+      <c r="G16" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" s="49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="23" customFormat="1" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="B17" s="21"/>
+      <c r="C17" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" s="49" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="26" customFormat="1" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="D17" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="22" t="s">
+      <c r="G17" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="J17" s="51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="38" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" s="22" t="s">
+      <c r="B18" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="G17" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="H17" s="25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="41" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="C18" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="D18" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="G18" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="I18" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="J18" s="49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="38" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="39" t="s">
+      <c r="B19" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="H18" s="42" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="41" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="39" t="s">
+      <c r="C19" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="D19" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="H19" s="42" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="G19" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="I19" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="J19" s="49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
bug report of v2
</commit_message>
<xml_diff>
--- a/IntegrationPlanning.xlsx
+++ b/IntegrationPlanning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Python-Hub\GithubRepos\Guru99-SW-Tesing-Project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023B414C-1F64-48EE-A3DD-DDFB6878A0E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C97597-1C5A-45F1-8A5C-D2728BD1E079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4110" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1762,7 +1762,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1780,7 +1780,7 @@
     <col min="11" max="16384" width="15.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Re-execution of intergration tests
Re-execution of integration tests
started making system tests
</commit_message>
<xml_diff>
--- a/IntegrationPlanning.xlsx
+++ b/IntegrationPlanning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Python-Hub\GithubRepos\Guru99-SW-Tesing-Project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C97597-1C5A-45F1-8A5C-D2728BD1E079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC8FCAC-C6FF-4D59-888E-47677E0AFA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4110" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="114">
   <si>
     <t>Date</t>
   </si>
@@ -42,12 +42,6 @@
   </si>
   <si>
     <t>Initial Draft</t>
-  </si>
-  <si>
-    <t>SR#</t>
-  </si>
-  <si>
-    <t>Test Scenario</t>
   </si>
   <si>
     <t>Test Cases</t>
@@ -75,19 +69,6 @@
 2) Submit</t>
   </si>
   <si>
-    <t>Sanjay
-Male
-24/02/1990
-Address - Ahmedabad
-City - Ahmedabad
-State - Gujarat
-PIN - 380009
-Telephone - 8000187025
-Email - sanjayrathod273@gmail.com
-UserId - 1234
-and submit</t>
-  </si>
-  <si>
     <t>Message Should be display "Customer added successfully !!"</t>
   </si>
   <si>
@@ -119,17 +100,6 @@
     <t>IP4</t>
   </si>
   <si>
-    <t>Verify Customer should not be edited for same email id and user id</t>
-  </si>
-  <si>
-    <t>Fill up all fields with repeated email and user id
-for example - Hirenwebdp@gmail.com is associate with userid - 1234
-then for edit other user (name - xyz ) hirenwebdp cannot be associate with user xyz</t>
-  </si>
-  <si>
-    <t>Message Should be display" customer records updated successfully!!"</t>
-  </si>
-  <si>
     <t>IP5</t>
   </si>
   <si>
@@ -140,9 +110,6 @@
 2) Submit</t>
   </si>
   <si>
-    <t>Customer Id = ABCD</t>
-  </si>
-  <si>
     <t>Message Should be display" You are not authorise to edit this customer!!"</t>
   </si>
   <si>
@@ -153,11 +120,6 @@
   </si>
   <si>
     <t>Check New account is added</t>
-  </si>
-  <si>
-    <t>customer id -1234
-account type-saving/current
-Initial Deposit-500</t>
   </si>
   <si>
     <t>Message Should be display " account
@@ -167,25 +129,13 @@
     <t>IP7</t>
   </si>
   <si>
-    <t>Verify that New Account is not added when same account id already exist</t>
-  </si>
-  <si>
-    <t>1) Enter all fields with customer id and account type already exist</t>
-  </si>
-  <si>
     <t>IP8</t>
-  </si>
-  <si>
-    <t>Check Ministatement is generated</t>
   </si>
   <si>
     <t>1) Enter Account Number
 2) Submit</t>
   </si>
   <si>
-    <t>Account Number - 360560330396</t>
-  </si>
-  <si>
     <t xml:space="preserve">Display Generated ministatement </t>
   </si>
   <si>
@@ -294,9 +244,6 @@
     <t xml:space="preserve">Displayed Generated ministatement </t>
   </si>
   <si>
-    <t>IP18</t>
-  </si>
-  <si>
     <t>Customized Statement</t>
   </si>
   <si>
@@ -337,23 +284,129 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>Not authourized</t>
-  </si>
-  <si>
     <t>Message displayed"Email address already exist"</t>
   </si>
   <si>
     <t>Account does not exist</t>
   </si>
   <si>
-    <t>You are not authorize to delete this customer!!</t>
+    <t>Test Title</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>mft
+Male
+1/1/2011
+Address - saas
+City - saas
+State - saas
+PIN - 999999
+Telephone - 0111111
+Email - sasa@haha.com
+and submit</t>
+  </si>
+  <si>
+    <t>ID: 36095</t>
+  </si>
+  <si>
+    <t>1) Enter Customer ID
+2) Submit
+3) Change one of the customer Fields</t>
+  </si>
+  <si>
+    <t>ID: 36095
+mobile number: 0222222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Customer Form is Opened with the fields already filled with already existing Customer data 
+after the changes were made, this message is displayed </t>
+  </si>
+  <si>
+    <t>Edit Customer Form is Opened with the fields already filled with already existing Customer data 
+after the changes were made, this message is displayed 
+But the changes were made anyway</t>
+  </si>
+  <si>
+    <t>new user name: wqwq
+new usew email: wqwq@haha.com</t>
+  </si>
+  <si>
+    <t>new user ID: 70200</t>
+  </si>
+  <si>
+    <t>Message Should be display" customer records cannot be updated"</t>
+  </si>
+  <si>
+    <t>1) Create a new customer with different records 
+1) edit the new customer name or email and use the first customer name or email
+2) Submit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer name Field cannot be changed, but Email is the same </t>
+  </si>
+  <si>
+    <t>Verify that 2 Customers should not have the same email id and user id</t>
+  </si>
+  <si>
+    <t>Customer Id = {any number that is not the one you got}</t>
+  </si>
+  <si>
+    <t>customer id - {use the one you got}
+account type-saving/current
+Initial Deposit-600</t>
+  </si>
+  <si>
+    <t>Account ID: 131806 for Customer ID:70200</t>
+  </si>
+  <si>
+    <t>1) Enter required fields
+2) Submit</t>
+  </si>
+  <si>
+    <t>1) Enter the same customer ID and account type as the previous Test Case
+2) Submit</t>
+  </si>
+  <si>
+    <t>customer id - {use the one you got}
+account type-saving/current
+Initial Deposit-700</t>
+  </si>
+  <si>
+    <t>Account ID: 131807 for Customer ID:70200</t>
+  </si>
+  <si>
+    <t>Customer Id - 1235</t>
+  </si>
+  <si>
+    <t>Connection Error</t>
+  </si>
+  <si>
+    <t>Blank Page, as there is no transactions yet
+" Can't confirm that the function is working correctly as no transaction scan be made in v2 "</t>
+  </si>
+  <si>
+    <t>Retest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">account number of an account that belongs to a deleted customer </t>
+  </si>
+  <si>
+    <t>Actual Result  v3</t>
+  </si>
+  <si>
+    <t>Pass/Fail v3</t>
+  </si>
+  <si>
+    <t>Verify that New Account is not added with the same account id already exist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -362,20 +415,24 @@
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -387,6 +444,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -406,8 +464,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -442,8 +507,13 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -537,15 +607,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -555,67 +616,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -633,12 +633,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -675,15 +676,6 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -708,97 +700,113 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -812,6 +820,876 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>311019</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>77754</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2301495</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>830135</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B8AFEA6-08C4-A206-1746-77FD3DC1AD76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14919259" y="485968"/>
+          <a:ext cx="1990476" cy="752381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>320739</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>106914</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2120739</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>687866</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C18993A-5FB0-FE8B-EECC-932AE1FA3FD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14928979" y="2303496"/>
+          <a:ext cx="1800000" cy="580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>240805</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1030257</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2089668</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1464403</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D325FB9-1094-5730-951D-C251BC003AE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14849045" y="5005487"/>
+          <a:ext cx="1848863" cy="434146"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>136072</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>359616</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1815758</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>97907</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00934B83-E52A-2AA9-F8CE-E583C0EFA4D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11604950" y="20206606"/>
+          <a:ext cx="4819048" cy="5171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>213828</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>194388</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2515284</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>709515</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5F88A9B-F7D4-709C-A983-A8D42AE0882A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14822068" y="6813291"/>
+          <a:ext cx="2301456" cy="515127"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>291581</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>48598</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1953597</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>683614</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{980A7557-BFD4-CB13-4933-32AAFAC8269C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14899821" y="7522807"/>
+          <a:ext cx="1662016" cy="635016"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>330459</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>48599</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1943878</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>631004</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32B4D1C5-3AC2-AA6D-41E2-CCF62AC19C58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14938699" y="8378114"/>
+          <a:ext cx="1613419" cy="582405"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>58317</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>165230</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2588753</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>738674</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D940FA30-3E2C-6154-604A-7F8600B8CECB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14666557" y="15337194"/>
+          <a:ext cx="2530436" cy="573444"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>330460</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>174949</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2139984</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>774949</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5175BD3-C8CB-A52F-35EF-E5D916C2E063}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14938700" y="10215077"/>
+          <a:ext cx="1809524" cy="600000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>369336</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>126352</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2173908</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>723812</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25859616-3923-3905-88DA-03140E4988FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14977576" y="17864235"/>
+          <a:ext cx="1804572" cy="597460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>311020</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>126352</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2115592</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>723812</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Picture 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30F9337C-8FC2-4585-1664-B7B3ED13A1D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14919260" y="11021786"/>
+          <a:ext cx="1804572" cy="597460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>126352</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>165229</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2002542</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>727134</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Picture 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D7CA8B8-5442-451C-5343-BF8213EF0381}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14734592" y="14481887"/>
+          <a:ext cx="1876190" cy="561905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>106913</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>126352</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1964056</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>764447</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Picture 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5643C0F7-BD78-CF8D-5E44-3EFA878A048F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14715153" y="16153622"/>
+          <a:ext cx="1857143" cy="638095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>427653</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>165230</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>736769</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1122023</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{791C7A4B-8F74-F3B7-4077-E6007FC9A473}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22004694" y="573444"/>
+          <a:ext cx="4352381" cy="4523809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>136071</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>369336</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1974166</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>978860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E95DDE2-374B-CFE7-A4EE-9940F0F39107}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18466836" y="2565918"/>
+          <a:ext cx="1838095" cy="609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>240805</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1030257</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1848863" cy="434146"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Picture 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EAD8FA8-3D12-4E23-8B9C-98B075C128BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14849045" y="5005487"/>
+          <a:ext cx="1848863" cy="434146"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>116634</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>213826</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2301456" cy="515127"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDB89DC9-9578-4A59-A526-953B10653D1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18447399" y="6832729"/>
+          <a:ext cx="2301456" cy="515127"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1302398</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>623461</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>586208</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Picture 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA60BEBF-B768-58A2-0668-8F0CF242FFFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22286556" y="5277628"/>
+          <a:ext cx="4190476" cy="3638095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>865025</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1341274</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>983664</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>663179</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Picture 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD8E04B7-65E0-0293-9378-9C64622C2410}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26718596" y="5316504"/>
+          <a:ext cx="4161905" cy="3676190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>330460</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>174949</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1809524" cy="600000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Picture 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA171E31-7550-4588-8B88-CE544529316F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14938700" y="10215077"/>
+          <a:ext cx="1809524" cy="600000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1225,10 +2103,10 @@
         <v>1</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1760,627 +2638,660 @@
   </sheetPr>
   <dimension ref="A1:T100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <pane xSplit="6" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="40" customWidth="1"/>
     <col min="2" max="2" width="13" style="14" customWidth="1"/>
     <col min="3" max="3" width="39.5703125" style="14" customWidth="1"/>
     <col min="4" max="4" width="38" style="14" customWidth="1"/>
     <col min="5" max="5" width="40.28515625" style="14" customWidth="1"/>
     <col min="6" max="6" width="33" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.5703125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="50" customWidth="1"/>
-    <col min="9" max="9" width="36.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" style="50" customWidth="1"/>
-    <col min="11" max="16384" width="15.140625" style="14"/>
+    <col min="7" max="7" width="29.28515625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="40" customWidth="1"/>
+    <col min="9" max="9" width="39.140625" style="14" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" style="40" customWidth="1"/>
+    <col min="11" max="11" width="37" style="14" customWidth="1"/>
+    <col min="12" max="16384" width="15.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:20" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="D1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="E1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="F1" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="G1" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+    </row>
+    <row r="2" spans="1:20" ht="141" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="B2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="H1" s="42" t="s">
+      <c r="C2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="18" customFormat="1" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="L3" s="39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="43" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J4" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="K4" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="F5" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="L5" s="26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="18" customFormat="1" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="19"/>
+      <c r="J6" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" s="19"/>
+      <c r="L6" s="30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" s="44" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="J7" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" s="22" customFormat="1" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="J8" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" s="43" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="J9" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="L9" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="K10" s="13"/>
+      <c r="L10" s="42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" s="18" customFormat="1" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" s="19"/>
+      <c r="J11" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="43" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="J13" s="39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" s="22" customFormat="1" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="J14" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" s="43" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" s="16"/>
+      <c r="J15" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" s="52" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="35"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="51"/>
+      <c r="J16" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="18" customFormat="1" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="I17" s="19"/>
+      <c r="J17" s="30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="48" customFormat="1" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="J18" s="53" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="48" customFormat="1" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="H19" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" s="25"/>
+      <c r="J19" s="29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="J20" s="49"/>
+    </row>
+    <row r="21" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H22" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-    </row>
-    <row r="2" spans="1:20" ht="141" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="H2" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="J2" s="45" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" s="23" customFormat="1" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="J3" s="51" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" s="26" customFormat="1" ht="141" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="H4" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="I4" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="J4" s="45" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="H5" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="I5" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="J5" s="49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" s="23" customFormat="1" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="H6" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="I6" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="J6" s="49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" s="30" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="H7" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="I7" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="J7" s="49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" s="31" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="H8" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="I8" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="J8" s="49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" s="35" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="H9" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="I9" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="J9" s="49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="H10" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="I10" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="J10" s="49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" s="23" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="H11" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="I11" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="J11" s="49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="H12" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="I12" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="J12" s="49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="H13" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="I13" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="J13" s="49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="H14" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="I14" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="J14" s="51" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" s="35" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="G15" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="H15" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="I15" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="J15" s="49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="H16" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="I16" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="J16" s="49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="23" customFormat="1" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="G17" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="H17" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="I17" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="J17" s="51" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="38" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="G18" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="H18" s="49" t="s">
-        <v>90</v>
-      </c>
-      <c r="I18" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="J18" s="49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="38" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="B19" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="C19" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="G19" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="H19" s="49" t="s">
-        <v>90</v>
-      </c>
-      <c r="I19" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="J19" s="49" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
     <row r="23" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2461,6 +3372,8 @@
     <row r="100" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <autoFilter ref="H1:H100" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>